<commit_message>
Updated Text to Image scripts added page wise testing so crsted 7 classes & each class having one test method & created common classes also
</commit_message>
<xml_diff>
--- a/TestDataGenerateImageAI/GenerateImage AI.xlsx
+++ b/TestDataGenerateImageAI/GenerateImage AI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mahipal\NYX.today\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591C13D1-0817-45F8-83D8-62E772251BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96DBAA3-6F46-4DDF-9BC6-4FDCDFE3872C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="382">
   <si>
     <t>Brand Name</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Innovating technology solutions that seamlessly integrate with your lifestyle.</t>
-  </si>
-  <si>
-    <t>Tech Enthusiasts</t>
   </si>
   <si>
     <t>Green Living Revolution</t>
@@ -1067,6 +1064,219 @@
   </si>
   <si>
     <t>Modern, stylish tech gadgets showcased in a minimalist, sleek environment with clean lines and an emphasis on innovation.</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Solar Water Heater</t>
+  </si>
+  <si>
+    <t>Modern rooftop solar water heater with sleek design, sunlit environment</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds</t>
+  </si>
+  <si>
+    <t>Compact wireless earbuds with charging case, minimalist design</t>
+  </si>
+  <si>
+    <t>Smartwatch</t>
+  </si>
+  <si>
+    <t>Stylish smartwatch with fitness tracking, notifications, heart-rate monitor</t>
+  </si>
+  <si>
+    <t>Gaming Laptop</t>
+  </si>
+  <si>
+    <t>High-performance gaming laptop with RGB keyboard, action-packed screen</t>
+  </si>
+  <si>
+    <t>Electric Bike</t>
+  </si>
+  <si>
+    <t>Sleek electric bike on city street, eco-friendly, futuristic design</t>
+  </si>
+  <si>
+    <t>Smart Thermostat</t>
+  </si>
+  <si>
+    <t>Smart thermostat on wall, modern home, temperature control display</t>
+  </si>
+  <si>
+    <t>DSLR Camera</t>
+  </si>
+  <si>
+    <t>Professional DSLR camera with lens, set against urban backdrop</t>
+  </si>
+  <si>
+    <t>VR Headset</t>
+  </si>
+  <si>
+    <t>Immersive VR headset with futuristic visuals, person enjoying virtual world</t>
+  </si>
+  <si>
+    <t>Noise-Canceling Headphones</t>
+  </si>
+  <si>
+    <t>Premium noise-canceling headphones, isolated in peaceful environment</t>
+  </si>
+  <si>
+    <t>Portable Bluetooth Speaker</t>
+  </si>
+  <si>
+    <t>Portable Bluetooth speaker on beach, outdoor party, rich sound</t>
+  </si>
+  <si>
+    <t>Smart Refrigerator</t>
+  </si>
+  <si>
+    <t>High-tech smart refrigerator in modern kitchen, touch display</t>
+  </si>
+  <si>
+    <t>Electric Scooter</t>
+  </si>
+  <si>
+    <t>Compact electric scooter zooming through busy city street, urban commuter</t>
+  </si>
+  <si>
+    <t>Wireless Charger</t>
+  </si>
+  <si>
+    <t>Sleek wireless charger on desk, phone charging, clutter-free space</t>
+  </si>
+  <si>
+    <t>Robot Vacuum Cleaner</t>
+  </si>
+  <si>
+    <t>Robot vacuum cleaner in clean, modern living room, autonomous cleaning</t>
+  </si>
+  <si>
+    <t>LED Desk Lamp</t>
+  </si>
+  <si>
+    <t>Adjustable LED desk lamp with modern design, perfect study lighting</t>
+  </si>
+  <si>
+    <t>Drone with Camera</t>
+  </si>
+  <si>
+    <t>Advanced drone with camera flying over scenic landscape, aerial photography</t>
+  </si>
+  <si>
+    <t>Electric Toothbrush</t>
+  </si>
+  <si>
+    <t>Modern electric toothbrush in bathroom, sleek and hygienic design</t>
+  </si>
+  <si>
+    <t>Smart Glasses</t>
+  </si>
+  <si>
+    <t>Futuristic smart glasses with AR display, urban environment</t>
+  </si>
+  <si>
+    <t>Fitness Tracker Band</t>
+  </si>
+  <si>
+    <t>Fitness tracker band on wrist, health and activity stats, workout scene</t>
+  </si>
+  <si>
+    <t>Wireless Mouse</t>
+  </si>
+  <si>
+    <t>Sleek wireless mouse on desk, ergonomic design, minimal clutter</t>
+  </si>
+  <si>
+    <t>Smart Home Hub</t>
+  </si>
+  <si>
+    <t>Smart home hub on table, controlling devices, futuristic living room</t>
+  </si>
+  <si>
+    <t>Electric Kettle</t>
+  </si>
+  <si>
+    <t>Stylish electric kettle in modern kitchen, water boiling, cozy atmosphere</t>
+  </si>
+  <si>
+    <t>Action Camera</t>
+  </si>
+  <si>
+    <t>Durable action camera on helmet, adventure sports, rugged terrain</t>
+  </si>
+  <si>
+    <t>Noise Machine</t>
+  </si>
+  <si>
+    <t>Portable noise machine on bedside table, soothing sleep sounds</t>
+  </si>
+  <si>
+    <t>Smart Mirror</t>
+  </si>
+  <si>
+    <t>Smart mirror in luxury bathroom, interactive display, virtual assistant</t>
+  </si>
+  <si>
+    <t>E-reader</t>
+  </si>
+  <si>
+    <t>Slim e-reader in cozy reading nook, warm light, digital pages</t>
+  </si>
+  <si>
+    <t>Standing Desk</t>
+  </si>
+  <si>
+    <t>Modern standing desk with dual monitors, ergonomic workspace setup</t>
+  </si>
+  <si>
+    <t>Air Purifier</t>
+  </si>
+  <si>
+    <t>Sleek air purifier in living room, clean air, minimalist design</t>
+  </si>
+  <si>
+    <t>Coffee Maker</t>
+  </si>
+  <si>
+    <t>High-tech coffee maker brewing fresh coffee, cozy kitchen scene</t>
+  </si>
+  <si>
+    <t>Smart Lock</t>
+  </si>
+  <si>
+    <t>Smart lock on front door, home security, modern entrance</t>
+  </si>
+  <si>
+    <t>Prompt(max 100 characters)</t>
+  </si>
+  <si>
+    <t>Tech Enthusiast</t>
+  </si>
+  <si>
+    <t>Product Image  Upload Selection(Use an asset or browse from system)</t>
+  </si>
+  <si>
+    <t>Use an Asset</t>
+  </si>
+  <si>
+    <t>Browse from System</t>
+  </si>
+  <si>
+    <t>SelectingImageBackdrops(prompt,Reference Image,Auto Generate)</t>
+  </si>
+  <si>
+    <t>Auto Generate</t>
+  </si>
+  <si>
+    <t>Browse from System Path</t>
+  </si>
+  <si>
+    <t>Reference Image Selection(Use an asset or Browse from system)</t>
+  </si>
+  <si>
+    <t>Reference Image Browse from system path</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1184,11 +1394,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1212,6 +1476,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1519,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1550,34 +1827,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>2</v>
@@ -1586,25 +1863,25 @@
         <v>3</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -1612,1491 +1889,1491 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="P2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="S2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>373</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
         <v>43</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="P3" s="5" t="s">
-        <v>236</v>
+        <v>31</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>222</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" t="s">
-        <v>223</v>
-      </c>
-      <c r="G4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="L4" s="10" t="s">
+      <c r="M4" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="N4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q4" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="R4" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="S4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G5" t="s">
+        <v>231</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>224</v>
-      </c>
-      <c r="G5" t="s">
-        <v>232</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="J5" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="M5" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="N5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>236</v>
+        <v>31</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="S5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" t="s">
+        <v>224</v>
+      </c>
+      <c r="G6" t="s">
+        <v>232</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="F6" t="s">
-        <v>225</v>
-      </c>
-      <c r="G6" t="s">
-        <v>233</v>
-      </c>
-      <c r="I6" s="10" t="s">
+      <c r="J6" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="L6" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="J6" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="L6" s="10" t="s">
+      <c r="M6" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="M6" s="10" t="s">
-        <v>65</v>
-      </c>
       <c r="N6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" t="s">
         <v>32</v>
       </c>
-      <c r="Q6" t="s">
-        <v>33</v>
-      </c>
       <c r="R6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="S6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="L7" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="L7" s="10" t="s">
+      <c r="M7" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="M7" s="10" t="s">
-        <v>70</v>
-      </c>
       <c r="N7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O7" t="s">
-        <v>268</v>
-      </c>
-      <c r="P7" t="s">
-        <v>236</v>
+        <v>267</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="Q7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="S7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>226</v>
+      </c>
+      <c r="G8" t="s">
+        <v>234</v>
+      </c>
+      <c r="I8" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>227</v>
-      </c>
-      <c r="G8" t="s">
-        <v>235</v>
-      </c>
-      <c r="I8" s="10" t="s">
+      <c r="J8" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="L8" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="L8" s="10" t="s">
+      <c r="M8" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="M8" s="10" t="s">
-        <v>75</v>
-      </c>
       <c r="N8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" t="s">
         <v>32</v>
       </c>
-      <c r="Q8" t="s">
-        <v>33</v>
-      </c>
       <c r="R8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="S8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F9" t="s">
+        <v>227</v>
+      </c>
+      <c r="G9" t="s">
+        <v>235</v>
+      </c>
+      <c r="I9" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="F9" t="s">
-        <v>228</v>
-      </c>
-      <c r="G9" t="s">
-        <v>236</v>
-      </c>
-      <c r="I9" s="10" t="s">
+      <c r="J9" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="L9" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="J9" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="L9" s="10" t="s">
+      <c r="M9" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="M9" s="10" t="s">
-        <v>81</v>
-      </c>
       <c r="N9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O9" t="s">
-        <v>266</v>
-      </c>
-      <c r="P9" t="s">
-        <v>236</v>
+        <v>265</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="Q9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>228</v>
+      </c>
+      <c r="G10" t="s">
+        <v>236</v>
+      </c>
+      <c r="I10" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>229</v>
-      </c>
-      <c r="G10" t="s">
-        <v>237</v>
-      </c>
-      <c r="I10" s="10" t="s">
+      <c r="J10" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="L10" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="J10" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="L10" s="10" t="s">
+      <c r="M10" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="M10" s="10" t="s">
-        <v>86</v>
-      </c>
       <c r="N10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P10" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10" t="s">
         <v>32</v>
       </c>
-      <c r="Q10" t="s">
-        <v>33</v>
-      </c>
       <c r="R10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="S10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>229</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" t="s">
-        <v>230</v>
-      </c>
-      <c r="G11" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="10" t="s">
+      <c r="J11" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="L11" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="L11" s="10" t="s">
+      <c r="M11" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="M11" s="10" t="s">
-        <v>91</v>
-      </c>
       <c r="N11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O11" t="s">
-        <v>267</v>
-      </c>
-      <c r="P11" t="s">
-        <v>236</v>
+        <v>266</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="Q11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="S11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>231</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" t="s">
-        <v>232</v>
-      </c>
-      <c r="I12" s="10" t="s">
+      <c r="J12" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="L12" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="J12" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="L12" s="10" t="s">
+      <c r="M12" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="M12" s="10" t="s">
-        <v>96</v>
-      </c>
       <c r="N12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" t="s">
         <v>32</v>
       </c>
-      <c r="Q12" t="s">
-        <v>33</v>
-      </c>
       <c r="R12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="S12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>230</v>
+      </c>
+      <c r="G13" t="s">
+        <v>232</v>
+      </c>
+      <c r="I13" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
-        <v>231</v>
-      </c>
-      <c r="G13" t="s">
-        <v>233</v>
-      </c>
-      <c r="I13" s="10" t="s">
+      <c r="J13" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="L13" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="J13" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="L13" s="10" t="s">
+      <c r="M13" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="M13" s="10" t="s">
-        <v>101</v>
-      </c>
       <c r="N13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O13" t="s">
+        <v>268</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q13" t="s">
         <v>269</v>
       </c>
-      <c r="P13" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>270</v>
-      </c>
       <c r="R13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="S13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>222</v>
+      </c>
+      <c r="G14" t="s">
+        <v>233</v>
+      </c>
+      <c r="I14" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" t="s">
-        <v>223</v>
-      </c>
-      <c r="G14" t="s">
-        <v>234</v>
-      </c>
-      <c r="I14" s="10" t="s">
+      <c r="J14" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="L14" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J14" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="L14" s="10" t="s">
+      <c r="M14" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="M14" s="10" t="s">
-        <v>106</v>
-      </c>
       <c r="N14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P14" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q14" t="s">
         <v>32</v>
       </c>
-      <c r="Q14" t="s">
-        <v>33</v>
-      </c>
       <c r="R14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="S14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D15" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
+        <v>223</v>
+      </c>
+      <c r="G15" t="s">
+        <v>234</v>
+      </c>
+      <c r="I15" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" t="s">
-        <v>224</v>
-      </c>
-      <c r="G15" t="s">
-        <v>235</v>
-      </c>
-      <c r="I15" s="10" t="s">
+      <c r="J15" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="L15" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="J15" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="L15" s="10" t="s">
+      <c r="M15" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="M15" s="10" t="s">
-        <v>111</v>
-      </c>
       <c r="N15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O15" t="s">
-        <v>45</v>
-      </c>
-      <c r="P15" t="s">
-        <v>236</v>
+        <v>44</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="Q15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="S15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
+        <v>224</v>
+      </c>
+      <c r="G16" t="s">
+        <v>235</v>
+      </c>
+      <c r="I16" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" t="s">
-        <v>225</v>
-      </c>
-      <c r="G16" t="s">
-        <v>236</v>
-      </c>
-      <c r="I16" s="10" t="s">
+      <c r="J16" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="L16" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="J16" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="L16" s="10" t="s">
+      <c r="M16" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="M16" s="10" t="s">
-        <v>117</v>
-      </c>
       <c r="N16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P16" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q16" t="s">
         <v>32</v>
       </c>
-      <c r="Q16" t="s">
-        <v>33</v>
-      </c>
       <c r="R16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="S16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D17" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>225</v>
+      </c>
+      <c r="G17" t="s">
+        <v>236</v>
+      </c>
+      <c r="I17" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" t="s">
-        <v>226</v>
-      </c>
-      <c r="G17" t="s">
-        <v>237</v>
-      </c>
-      <c r="I17" s="10" t="s">
+      <c r="J17" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="L17" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="J17" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="L17" s="10" t="s">
+      <c r="M17" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="M17" s="10" t="s">
-        <v>122</v>
-      </c>
       <c r="N17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O17" t="s">
-        <v>268</v>
-      </c>
-      <c r="P17" t="s">
-        <v>236</v>
+        <v>267</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="Q17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="S17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>226</v>
+      </c>
+      <c r="G18" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" t="s">
-        <v>227</v>
-      </c>
-      <c r="G18" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" s="10" t="s">
+      <c r="J18" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="L18" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="J18" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="L18" s="10" t="s">
+      <c r="M18" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="M18" s="10" t="s">
-        <v>127</v>
-      </c>
       <c r="N18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q18" t="s">
         <v>32</v>
       </c>
-      <c r="Q18" t="s">
-        <v>33</v>
-      </c>
       <c r="R18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="S18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D19" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F19" t="s">
+        <v>227</v>
+      </c>
+      <c r="G19" t="s">
+        <v>231</v>
+      </c>
+      <c r="I19" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="F19" t="s">
-        <v>228</v>
-      </c>
-      <c r="G19" t="s">
-        <v>232</v>
-      </c>
-      <c r="I19" s="10" t="s">
+      <c r="J19" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="L19" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="J19" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="L19" s="10" t="s">
+      <c r="M19" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="M19" s="10" t="s">
-        <v>132</v>
-      </c>
       <c r="N19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O19" t="s">
-        <v>266</v>
-      </c>
-      <c r="P19" t="s">
-        <v>236</v>
+        <v>265</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="Q19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D20" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G20" t="s">
+        <v>232</v>
+      </c>
+      <c r="I20" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" t="s">
-        <v>229</v>
-      </c>
-      <c r="G20" t="s">
-        <v>233</v>
-      </c>
-      <c r="I20" s="10" t="s">
+      <c r="J20" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="L20" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="J20" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="L20" s="10" t="s">
+      <c r="M20" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="M20" s="10" t="s">
-        <v>137</v>
-      </c>
       <c r="N20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P20" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" t="s">
         <v>32</v>
       </c>
-      <c r="Q20" t="s">
-        <v>33</v>
-      </c>
       <c r="R20" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D21" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" t="s">
+        <v>229</v>
+      </c>
+      <c r="G21" t="s">
+        <v>233</v>
+      </c>
+      <c r="I21" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" t="s">
-        <v>230</v>
-      </c>
-      <c r="G21" t="s">
-        <v>234</v>
-      </c>
-      <c r="I21" s="10" t="s">
+      <c r="J21" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="L21" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="J21" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="L21" s="10" t="s">
+      <c r="M21" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="M21" s="10" t="s">
-        <v>142</v>
-      </c>
       <c r="N21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O21" t="s">
-        <v>267</v>
-      </c>
-      <c r="P21" t="s">
-        <v>236</v>
+        <v>266</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="Q21" t="s">
+        <v>269</v>
+      </c>
+      <c r="R21" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="R21" s="5" t="s">
-        <v>271</v>
-      </c>
       <c r="S21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D22" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" t="s">
+        <v>234</v>
+      </c>
+      <c r="I22" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" t="s">
-        <v>235</v>
-      </c>
-      <c r="I22" s="10" t="s">
+      <c r="J22" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="L22" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="J22" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="L22" s="10" t="s">
+      <c r="M22" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="M22" s="10" t="s">
-        <v>147</v>
-      </c>
       <c r="N22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P22" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q22" t="s">
         <v>32</v>
       </c>
-      <c r="Q22" t="s">
-        <v>33</v>
-      </c>
       <c r="R22" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="S22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D23" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" t="s">
+        <v>226</v>
+      </c>
+      <c r="G23" t="s">
+        <v>235</v>
+      </c>
+      <c r="I23" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" t="s">
-        <v>227</v>
-      </c>
-      <c r="G23" t="s">
-        <v>236</v>
-      </c>
-      <c r="I23" s="10" t="s">
+      <c r="J23" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="L23" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="J23" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="L23" s="10" t="s">
+      <c r="M23" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="M23" s="10" t="s">
-        <v>152</v>
-      </c>
       <c r="N23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O23" t="s">
+        <v>268</v>
+      </c>
+      <c r="P23" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q23" t="s">
         <v>269</v>
       </c>
-      <c r="P23" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>270</v>
-      </c>
       <c r="R23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="S23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D24" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
+        <v>227</v>
+      </c>
+      <c r="G24" t="s">
+        <v>236</v>
+      </c>
+      <c r="I24" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" t="s">
-        <v>228</v>
-      </c>
-      <c r="G24" t="s">
-        <v>237</v>
-      </c>
-      <c r="I24" s="10" t="s">
+      <c r="J24" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="L24" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="J24" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="L24" s="10" t="s">
+      <c r="M24" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="M24" s="10" t="s">
-        <v>157</v>
-      </c>
       <c r="N24" t="s">
+        <v>264</v>
+      </c>
+      <c r="O24" t="s">
         <v>265</v>
       </c>
-      <c r="O24" t="s">
-        <v>266</v>
-      </c>
       <c r="P24" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q24" t="s">
         <v>32</v>
       </c>
-      <c r="Q24" t="s">
-        <v>33</v>
-      </c>
       <c r="R24" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="S24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D25" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F25" t="s">
+        <v>228</v>
+      </c>
+      <c r="G25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="L25" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="F25" t="s">
-        <v>229</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="M25" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="N25" t="s">
+        <v>264</v>
+      </c>
+      <c r="O25" t="s">
         <v>44</v>
       </c>
-      <c r="I25" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="L25" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="M25" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="N25" t="s">
-        <v>265</v>
-      </c>
-      <c r="O25" t="s">
-        <v>45</v>
-      </c>
       <c r="P25" t="s">
-        <v>236</v>
+        <v>31</v>
       </c>
       <c r="Q25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="S25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D26" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" t="s">
+        <v>229</v>
+      </c>
+      <c r="G26" t="s">
+        <v>231</v>
+      </c>
+      <c r="I26" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" t="s">
-        <v>230</v>
-      </c>
-      <c r="G26" t="s">
-        <v>232</v>
-      </c>
-      <c r="I26" s="10" t="s">
+      <c r="J26" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="L26" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="J26" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="L26" s="10" t="s">
+      <c r="M26" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="M26" s="10" t="s">
-        <v>166</v>
-      </c>
       <c r="N26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="O26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P26" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q26" t="s">
         <v>32</v>
       </c>
-      <c r="Q26" t="s">
-        <v>33</v>
-      </c>
       <c r="R26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D27" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" t="s">
+        <v>232</v>
+      </c>
+      <c r="I27" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" t="s">
-        <v>43</v>
-      </c>
-      <c r="G27" t="s">
-        <v>233</v>
-      </c>
-      <c r="I27" s="10" t="s">
+      <c r="J27" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="L27" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="J27" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="L27" s="10" t="s">
-        <v>170</v>
-      </c>
       <c r="M27" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N27" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="O27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P27" t="s">
-        <v>236</v>
+        <v>31</v>
       </c>
       <c r="Q27" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R27" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="S27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D28" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" t="s">
+        <v>230</v>
+      </c>
+      <c r="G28" t="s">
+        <v>233</v>
+      </c>
+      <c r="I28" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="E28" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" t="s">
-        <v>231</v>
-      </c>
-      <c r="G28" t="s">
-        <v>234</v>
-      </c>
-      <c r="I28" s="10" t="s">
+      <c r="J28" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="L28" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="J28" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="L28" s="10" t="s">
-        <v>174</v>
-      </c>
       <c r="M28" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="O28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P28" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q28" t="s">
         <v>32</v>
       </c>
-      <c r="Q28" t="s">
-        <v>33</v>
-      </c>
       <c r="R28" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="S28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D29" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" t="s">
+        <v>222</v>
+      </c>
+      <c r="G29" t="s">
+        <v>234</v>
+      </c>
+      <c r="I29" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" t="s">
-        <v>223</v>
-      </c>
-      <c r="G29" t="s">
-        <v>235</v>
-      </c>
-      <c r="I29" s="10" t="s">
+      <c r="J29" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="L29" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="J29" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="L29" s="10" t="s">
-        <v>178</v>
-      </c>
       <c r="M29" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O29" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P29" t="s">
-        <v>236</v>
+        <v>31</v>
       </c>
       <c r="Q29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="R29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="S29" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
@@ -3110,26 +3387,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="40.109375" customWidth="1"/>
-    <col min="17" max="17" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.5546875" customWidth="1"/>
+    <col min="6" max="6" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="40.109375" customWidth="1"/>
+    <col min="20" max="20" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+    <row r="1" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>381</v>
+      </c>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
@@ -3140,15 +3438,26 @@
       <c r="O1" s="9"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+    </row>
+    <row r="2" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -3159,15 +3468,26 @@
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -3178,15 +3498,24 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
@@ -3197,15 +3526,24 @@
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -3216,15 +3554,24 @@
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -3235,15 +3582,24 @@
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -3254,15 +3610,24 @@
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -3273,15 +3638,22 @@
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -3292,15 +3664,22 @@
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+    </row>
+    <row r="10" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -3311,15 +3690,22 @@
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+    </row>
+    <row r="11" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -3330,15 +3716,22 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+    </row>
+    <row r="12" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
@@ -3349,15 +3742,22 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -3368,15 +3768,22 @@
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
@@ -3387,15 +3794,22 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+    </row>
+    <row r="15" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -3406,15 +3820,22 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -3425,15 +3846,22 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+    </row>
+    <row r="17" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
@@ -3444,15 +3872,22 @@
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+    </row>
+    <row r="18" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
@@ -3463,15 +3898,22 @@
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
@@ -3482,15 +3924,22 @@
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+    </row>
+    <row r="20" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
@@ -3501,15 +3950,22 @@
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
@@ -3520,15 +3976,22 @@
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
@@ -3539,15 +4002,22 @@
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
@@ -3558,15 +4028,22 @@
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
@@ -3577,15 +4054,22 @@
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
@@ -3596,15 +4080,22 @@
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
@@ -3615,15 +4106,22 @@
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
@@ -3634,6 +4132,61 @@
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15" t="s">
+        <v>365</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Save work before switching to master
</commit_message>
<xml_diff>
--- a/TestDataGenerateImageAI/GenerateImage AI.xlsx
+++ b/TestDataGenerateImageAI/GenerateImage AI.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mahipal\NYX.today\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96DBAA3-6F46-4DDF-9BC6-4FDCDFE3872C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C32F84-2221-4259-AB93-5FAB34BE0F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="LogIn" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="421">
   <si>
     <t>Brand Name</t>
   </si>
@@ -1277,13 +1279,130 @@
   </si>
   <si>
     <t>Reference Image Browse from system path</t>
+  </si>
+  <si>
+    <t>D:\Mahipal\NYX.today\ProductLogo\Bamboo.png</t>
+  </si>
+  <si>
+    <t>AI Prompt</t>
+  </si>
+  <si>
+    <t>Script (AI Prompt,Your Script)</t>
+  </si>
+  <si>
+    <t>Your Script</t>
+  </si>
+  <si>
+    <t>Video Structure (AI Images (Photorealistic), Stock Images,Stock Videos,AI Images (Art))</t>
+  </si>
+  <si>
+    <t>AI Images (Photorealistic)</t>
+  </si>
+  <si>
+    <t>Video Size (Square, Landscape, Potrait, Story, Pin)</t>
+  </si>
+  <si>
+    <t>Square</t>
+  </si>
+  <si>
+    <t>Pace (Fast, Medium, Slow)</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Captions (Hide Captions, Show Captions)</t>
+  </si>
+  <si>
+    <t>Hide Captions</t>
+  </si>
+  <si>
+    <t>Start Slate Image Upload</t>
+  </si>
+  <si>
+    <t>End Slate Image Upload</t>
+  </si>
+  <si>
+    <t>Playing Cricket</t>
+  </si>
+  <si>
+    <t>Writing Style(Casual, Dramatic, Neutral, Informative, Funny, Persuasive, Engaging, Professional)</t>
+  </si>
+  <si>
+    <t>Casual</t>
+  </si>
+  <si>
+    <t>Duration(1,2,3,4,…,29,30)</t>
+  </si>
+  <si>
+    <t>Slate Selection(Start Slate, End Slate, Both)</t>
+  </si>
+  <si>
+    <t>Start Slate</t>
+  </si>
+  <si>
+    <t>D:\Mahipal\NYX.today\BrandLogos\EcoBlend.png</t>
+  </si>
+  <si>
+    <t>UploadFileSelection(Upload from Drive, Broswe from System)</t>
+  </si>
+  <si>
+    <t>Animaation Style Selection(Vertical, Horizontal, Zoom In, Zoom Out, Zoom Left, Zoom Right, Perspective, Circle, Dolly)</t>
+  </si>
+  <si>
+    <t>Vertical</t>
+  </si>
+  <si>
+    <t>Amount of motion(1 to 100) in percentage</t>
+  </si>
+  <si>
+    <t>Animation Duration(0 to 6 sec)</t>
+  </si>
+  <si>
+    <t>CountryCode</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>wrongpass</t>
+  </si>
+  <si>
+    <t>Failure</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>abcdefg</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>special$$</t>
+  </si>
+  <si>
+    <t>Nyx.today1234</t>
+  </si>
+  <si>
+    <t>IN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1306,6 +1425,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFDEE4E4"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFE3E3E3"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1452,7 +1583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1489,6 +1620,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1796,8 +1939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3389,15 +3532,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="67.5546875" customWidth="1"/>
     <col min="6" max="6" width="22.21875" bestFit="1" customWidth="1"/>
@@ -3447,9 +3590,11 @@
         <v>312</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>375</v>
-      </c>
-      <c r="C2" s="14"/>
+        <v>376</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>382</v>
+      </c>
       <c r="D2" s="14" t="s">
         <v>378</v>
       </c>
@@ -4195,12 +4340,418 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="69.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="53.6640625" customWidth="1"/>
+    <col min="15" max="16" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="79.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="72.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="72.109375" customWidth="1"/>
+    <col min="24" max="24" width="45.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="72.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>383</v>
+      </c>
+      <c r="O2" t="s">
+        <v>396</v>
+      </c>
+      <c r="P2" t="s">
+        <v>396</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>398</v>
+      </c>
+      <c r="R2">
+        <v>20</v>
+      </c>
+      <c r="S2" t="s">
+        <v>387</v>
+      </c>
+      <c r="T2" t="s">
+        <v>389</v>
+      </c>
+      <c r="U2" t="s">
+        <v>391</v>
+      </c>
+      <c r="V2" t="s">
+        <v>393</v>
+      </c>
+      <c r="W2" t="s">
+        <v>401</v>
+      </c>
+      <c r="X2" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="P8" s="20"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="U15" s="19"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64C0924-1A73-4704-A449-DF638D22E33F}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393D9961-F31F-4DCA-A2EF-887B964485C5}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>408</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B2" s="24">
+        <v>7204439138</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B3" s="24">
+        <v>1234567890</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B4" s="24">
+        <v>123</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B5" s="24">
+        <v>72044391381234</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B7" s="24">
+        <v>9876543210</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B8" s="24">
+        <v>9876543210</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B10" s="24">
+        <v>9876543210</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
To run script in production for text to images script modified
</commit_message>
<xml_diff>
--- a/TestDataGenerateImageAI/GenerateImage AI.xlsx
+++ b/TestDataGenerateImageAI/GenerateImage AI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mahipal\NYX.today\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C32F84-2221-4259-AB93-5FAB34BE0F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBEB98F-5FF0-4035-A04D-AF6AA0D6C965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="421">
   <si>
     <t>Brand Name</t>
   </si>
@@ -1281,9 +1281,6 @@
     <t>Reference Image Browse from system path</t>
   </si>
   <si>
-    <t>D:\Mahipal\NYX.today\ProductLogo\Bamboo.png</t>
-  </si>
-  <si>
     <t>AI Prompt</t>
   </si>
   <si>
@@ -1396,6 +1393,9 @@
   </si>
   <si>
     <t>IN</t>
+  </si>
+  <si>
+    <t>D:\Mahipal\NYX.today\BrandLogos\Gas bill.jpg</t>
   </si>
 </sst>
 </file>
@@ -3532,8 +3532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3593,7 +3593,7 @@
         <v>376</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>382</v>
+        <v>420</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>378</v>
@@ -4412,40 +4412,40 @@
         <v>3</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>400</v>
-      </c>
       <c r="X1" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="Z1" s="8" t="s">
         <v>20</v>
@@ -4492,40 +4492,40 @@
         <v>11</v>
       </c>
       <c r="N2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="P2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R2">
         <v>20</v>
       </c>
       <c r="S2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="T2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="U2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="V2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="W2" t="s">
+        <v>400</v>
+      </c>
+      <c r="X2" t="s">
         <v>401</v>
       </c>
-      <c r="X2" t="s">
-        <v>402</v>
-      </c>
       <c r="Y2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
@@ -4557,16 +4557,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>404</v>
-      </c>
       <c r="C1" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>406</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4574,7 +4574,7 @@
         <v>376</v>
       </c>
       <c r="B2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -4592,7 +4592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393D9961-F31F-4DCA-A2EF-887B964485C5}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -4606,148 +4606,148 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>408</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>409</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="D1" s="22" t="s">
         <v>410</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B2" s="24">
         <v>7204439138</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B3" s="24">
         <v>1234567890</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>413</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B4" s="24">
         <v>123</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B5" s="24">
         <v>72044391381234</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B7" s="24">
         <v>9876543210</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B8" s="24">
         <v>9876543210</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B10" s="24">
         <v>9876543210</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more time for image generation
</commit_message>
<xml_diff>
--- a/TestDataGenerateImageAI/GenerateImage AI.xlsx
+++ b/TestDataGenerateImageAI/GenerateImage AI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mahipal\NYX.today\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBEB98F-5FF0-4035-A04D-AF6AA0D6C965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3234F810-D290-43FF-8D16-7758937B0F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="421">
   <si>
     <t>Brand Name</t>
   </si>
@@ -3533,7 +3533,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3590,7 +3590,7 @@
         <v>312</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>420</v>
@@ -3791,7 +3791,9 @@
       <c r="A9" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="B9" s="14"/>
+      <c r="B9" s="14" t="s">
+        <v>376</v>
+      </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">

</xml_diff>

<commit_message>
Changed as per Production requirement
</commit_message>
<xml_diff>
--- a/TestDataGenerateImageAI/GenerateImage AI.xlsx
+++ b/TestDataGenerateImageAI/GenerateImage AI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mahipal\NYX.today\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754E5891-E6B6-4066-B016-99B333EFE491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF738700-3FC7-4938-A1DF-E5E1D726C9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4564,8 +4564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64C0924-1A73-4704-A449-DF638D22E33F}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>